<commit_message>
GIải thích nô bộc
</commit_message>
<xml_diff>
--- a/LuanNoBoc.xlsx
+++ b/LuanNoBoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77B090F-11B1-4720-8039-FA4E7685540E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9876C59F-6030-4E91-9035-7269EA1C386D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15168" uniqueCount="6520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15168" uniqueCount="6522">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -19586,6 +19586,12 @@
   </si>
   <si>
     <t>Tham Lang sao tối toạ thủ tại Mệnh gặp Thiên Phủ ở Huynh Đệ sao tối</t>
+  </si>
+  <si>
+    <t>Bạn bè có danh chức.</t>
+  </si>
+  <si>
+    <t>Bạn bè nhiều người giỏi</t>
   </si>
 </sst>
 </file>
@@ -19630,67 +19636,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="33">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -20300,8 +20246,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B6523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5437" workbookViewId="0">
-      <selection activeCell="F5450" sqref="F5450"/>
+    <sheetView tabSelected="1" topLeftCell="A318" workbookViewId="0">
+      <selection activeCell="D325" sqref="D325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54050,7 +53996,7 @@
         <v>4217</v>
       </c>
       <c r="B4220" s="1" t="s">
-        <v>4217</v>
+        <v>6521</v>
       </c>
     </row>
     <row r="4221" spans="1:2" x14ac:dyDescent="0.25">
@@ -54506,7 +54452,7 @@
         <v>4274</v>
       </c>
       <c r="B4277" s="1" t="s">
-        <v>4274</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="4278" spans="1:2" x14ac:dyDescent="0.25">
@@ -72472,68 +72418,68 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="38" priority="101"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="102"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="36" priority="71"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="71"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="34" priority="75"/>
-    <cfRule type="duplicateValues" dxfId="33" priority="76"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="76"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="32" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="70"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1810:A3339">
+    <cfRule type="duplicateValues" dxfId="25" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3814:A3875">
+    <cfRule type="duplicateValues" dxfId="24" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4981:A5459 A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3813 A3876:A4176 A6524:A1048576">
-    <cfRule type="duplicateValues" dxfId="31" priority="110"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="112"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="110"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="112"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="29" priority="53"/>
+  <conditionalFormatting sqref="A6045:A6523">
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3814:A3875">
-    <cfRule type="duplicateValues" dxfId="28" priority="32"/>
+  <conditionalFormatting sqref="A1:B5459 A6524:B1048576">
+    <cfRule type="duplicateValues" dxfId="19" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5460:B6523">
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="27" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="21" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1810:B3339">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3814:B3875">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4981:B5459 B209:B1631 B1:B23 B25:B84 B143 B1805:B1809 B3442:B3813 B3876:B4176 B6524:B1048576">
-    <cfRule type="duplicateValues" dxfId="20" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B3339">
-    <cfRule type="duplicateValues" dxfId="18" priority="11"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3814:B3875">
-    <cfRule type="duplicateValues" dxfId="17" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B5459 A6524:B1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6045:A6523">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6045:B6523">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5460:B6523">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -81064,15 +81010,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A586:A1064">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:B1064">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B586:B1064">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:B1064">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Giải thích thiên cơ
</commit_message>
<xml_diff>
--- a/LuanNoBoc.xlsx
+++ b/LuanNoBoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707D1978-F468-4620-80BE-4DB9DEBDA64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BFFA59-FC98-42D1-A5A2-4791855FA5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10695" uniqueCount="4451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10695" uniqueCount="4452">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13386,6 +13386,9 @@
   </si>
   <si>
     <t>Khuyết điểm: Nhiều mơ ước ấu trĩ. Thiếu tự tin, không dám biểu lộ quan điểm riêng của mình. Cách suy nghĩ cũng như hành động đều bất định. Lý trí yếu, không đủ kềm hãm con tim; dễ bị thua thiệt trong tình cảm. Thiếu khả năng lãnh đạo, điều hợp. Không thể đảm nhận việc quan trọng.</t>
+  </si>
+  <si>
+    <t>Mang lụy vì tình, ưa việc trăng gió, bướm hoa.</t>
   </si>
 </sst>
 </file>
@@ -13436,7 +13439,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13766,8 +13779,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:G4262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4222" workbookViewId="0">
-      <selection activeCell="C4229" sqref="C4229"/>
+    <sheetView tabSelected="1" topLeftCell="A4240" workbookViewId="0">
+      <selection activeCell="A3367" sqref="A3367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17367,7 +17380,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="451" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>493</v>
       </c>
@@ -17375,7 +17388,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="452" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>494</v>
       </c>
@@ -25823,7 +25836,7 @@
         <v>1528</v>
       </c>
     </row>
-    <row r="1508" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1508" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1508" s="1" t="s">
         <v>1529</v>
       </c>
@@ -29372,7 +29385,7 @@
         <v>1947</v>
       </c>
       <c r="B1951" s="1" t="s">
-        <v>1947</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="1952" spans="1:2" x14ac:dyDescent="0.25">
@@ -48016,6 +48029,9 @@
   </sheetData>
   <autoFilter ref="A2:D4261" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -56545,15 +56561,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A586:A1064">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B1064">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B586:B1064">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>